<commit_message>
Added extruded map in deck.gl
</commit_message>
<xml_diff>
--- a/assets/data/Refugee_Flows/data/Total.xlsx
+++ b/assets/data/Refugee_Flows/data/Total.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Giovanni\SynologyDrive\refugee\assets\data\Refugee_Flows\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3F9F656-0A47-4834-ACE8-3EEE0DC02BB8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D65EA09-3604-43E8-AE26-2B6BC3004FF4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11625" activeTab="4" xr2:uid="{200C97B3-33C3-4ACD-A66F-46BCD538826D}"/>
   </bookViews>
@@ -1170,9 +1170,6 @@
     <t>NOR</t>
   </si>
   <si>
-    <t>PSE</t>
-  </si>
-  <si>
     <t>OMN</t>
   </si>
   <si>
@@ -1335,9 +1332,6 @@
     <t>VNM</t>
   </si>
   <si>
-    <t>WLF</t>
-  </si>
-  <si>
     <t>YEM</t>
   </si>
   <si>
@@ -1351,6 +1345,12 @@
   </si>
   <si>
     <t>ISO</t>
+  </si>
+  <si>
+    <t>PSX</t>
+  </si>
+  <si>
+    <t>SAH</t>
   </si>
 </sst>
 </file>
@@ -10608,7 +10608,7 @@
   <dimension ref="A1:D179"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A151" workbookViewId="0">
-      <selection activeCell="D159" sqref="D159"/>
+      <selection activeCell="E174" sqref="E174"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -10630,7 +10630,7 @@
         <v>257</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -12301,7 +12301,7 @@
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" s="7" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B121" s="5">
         <v>421</v>
@@ -12310,7 +12310,7 @@
         <v>1765</v>
       </c>
       <c r="D121" s="16" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
@@ -12338,7 +12338,7 @@
         <v>38</v>
       </c>
       <c r="D123" s="16" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
@@ -12352,7 +12352,7 @@
         <v>134633</v>
       </c>
       <c r="D124" s="16" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
@@ -12366,7 +12366,7 @@
         <v>47</v>
       </c>
       <c r="D125" s="16" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
@@ -12380,7 +12380,7 @@
         <v>430</v>
       </c>
       <c r="D126" s="16" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
@@ -12394,7 +12394,7 @@
         <v>77</v>
       </c>
       <c r="D127" s="16" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
@@ -12408,7 +12408,7 @@
         <v>2582</v>
       </c>
       <c r="D128" s="16" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
@@ -12422,7 +12422,7 @@
         <v>490</v>
       </c>
       <c r="D129" s="16" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
@@ -12436,7 +12436,7 @@
         <v>1085</v>
       </c>
       <c r="D130" s="16" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
@@ -12450,7 +12450,7 @@
         <v>18</v>
       </c>
       <c r="D131" s="16" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
@@ -12464,7 +12464,7 @@
         <v>35</v>
       </c>
       <c r="D132" s="16" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
@@ -12478,7 +12478,7 @@
         <v>242</v>
       </c>
       <c r="D133" s="16" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
@@ -12492,7 +12492,7 @@
         <v>1217</v>
       </c>
       <c r="D134" s="16" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
@@ -12506,7 +12506,7 @@
         <v>61934</v>
       </c>
       <c r="D135" s="16" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
@@ -12520,7 +12520,7 @@
         <v>248698</v>
       </c>
       <c r="D136" s="16" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
@@ -12534,7 +12534,7 @@
         <v>1009</v>
       </c>
       <c r="D137" s="16" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
@@ -12548,7 +12548,7 @@
         <v>1279</v>
       </c>
       <c r="D138" s="16" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
@@ -12562,7 +12562,7 @@
         <v>1394</v>
       </c>
       <c r="D139" s="16" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
@@ -12576,7 +12576,7 @@
         <v>28165</v>
       </c>
       <c r="D140" s="16" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
@@ -12590,7 +12590,7 @@
         <v>32983</v>
       </c>
       <c r="D141" s="16" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
@@ -12604,7 +12604,7 @@
         <v>4732</v>
       </c>
       <c r="D142" s="16" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
@@ -12618,7 +12618,7 @@
         <v>48</v>
       </c>
       <c r="D143" s="16" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
@@ -12632,7 +12632,7 @@
         <v>1090</v>
       </c>
       <c r="D144" s="16" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
@@ -12646,7 +12646,7 @@
         <v>21</v>
       </c>
       <c r="D145" s="16" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
@@ -12660,7 +12660,7 @@
         <v>954701</v>
       </c>
       <c r="D146" s="16" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
@@ -12674,7 +12674,7 @@
         <v>476</v>
       </c>
       <c r="D147" s="16" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
@@ -12688,7 +12688,7 @@
         <v>2214595</v>
       </c>
       <c r="D148" s="18" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
@@ -12702,7 +12702,7 @@
         <v>45</v>
       </c>
       <c r="D149" s="16" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
@@ -12716,7 +12716,7 @@
         <v>114602</v>
       </c>
       <c r="D150" s="16" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
@@ -12730,7 +12730,7 @@
         <v>719222</v>
       </c>
       <c r="D151" s="16" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
@@ -12744,7 +12744,7 @@
         <v>19</v>
       </c>
       <c r="D152" s="16" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
@@ -12758,7 +12758,7 @@
         <v>238</v>
       </c>
       <c r="D153" s="16" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
@@ -12772,7 +12772,7 @@
         <v>20</v>
       </c>
       <c r="D154" s="16" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
@@ -12786,7 +12786,7 @@
         <v>0</v>
       </c>
       <c r="D155" s="16" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
@@ -12800,7 +12800,7 @@
         <v>6490950</v>
       </c>
       <c r="D156" s="16" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
@@ -12814,7 +12814,7 @@
         <v>1596</v>
       </c>
       <c r="D157" s="16" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
@@ -12828,7 +12828,7 @@
         <v>179</v>
       </c>
       <c r="D158" s="16" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
@@ -12842,7 +12842,7 @@
         <v>8149</v>
       </c>
       <c r="D159" s="16" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
@@ -12856,7 +12856,7 @@
         <v>313</v>
       </c>
       <c r="D160" s="16" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
@@ -12870,7 +12870,7 @@
         <v>1931</v>
       </c>
       <c r="D161" s="16" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
@@ -12884,7 +12884,7 @@
         <v>65754</v>
       </c>
       <c r="D162" s="16" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
@@ -12898,7 +12898,7 @@
         <v>414</v>
       </c>
       <c r="D163" s="16" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
@@ -12912,7 +12912,7 @@
         <v>16</v>
       </c>
       <c r="D164" s="16" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
@@ -12926,7 +12926,7 @@
         <v>6630</v>
       </c>
       <c r="D165" s="16" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
@@ -12940,7 +12940,7 @@
         <v>119832</v>
       </c>
       <c r="D166" s="16" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
@@ -12954,12 +12954,12 @@
         <v>161</v>
       </c>
       <c r="D167" s="16" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="168" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A168" s="20" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B168" s="5">
         <v>124018</v>
@@ -12968,7 +12968,7 @@
         <v>84</v>
       </c>
       <c r="D168" s="16" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
@@ -12982,7 +12982,7 @@
         <v>724</v>
       </c>
       <c r="D169" s="16" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
@@ -12996,7 +12996,7 @@
         <v>322</v>
       </c>
       <c r="D170" s="16" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
@@ -13010,7 +13010,7 @@
         <v>19</v>
       </c>
       <c r="D171" s="16" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
@@ -13024,7 +13024,7 @@
         <v>3380</v>
       </c>
       <c r="D172" s="16" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
@@ -13038,7 +13038,7 @@
         <v>12664</v>
       </c>
       <c r="D173" s="16" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
@@ -13052,7 +13052,7 @@
         <v>334317</v>
       </c>
       <c r="D174" s="16" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
@@ -13066,7 +13066,7 @@
         <v>101125</v>
       </c>
       <c r="D175" s="16" t="s">
-        <v>433</v>
+        <v>437</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
@@ -13080,7 +13080,7 @@
         <v>200333</v>
       </c>
       <c r="D176" s="16" t="s">
-        <v>378</v>
+        <v>438</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
@@ -13094,7 +13094,7 @@
         <v>26793</v>
       </c>
       <c r="D177" s="16" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
@@ -13108,7 +13108,7 @@
         <v>283</v>
       </c>
       <c r="D178" s="16" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
@@ -13122,7 +13122,7 @@
         <v>16482</v>
       </c>
       <c r="D179" s="17" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
     </row>
   </sheetData>

</xml_diff>